<commit_message>
Updated all the Excel files
</commit_message>
<xml_diff>
--- a/Legend-for-Categorical-Variables.xlsx
+++ b/Legend-for-Categorical-Variables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joash\Desktop\University Stuff\3B Uni Stuff\MSCI 446\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joash\PycharmProjects\Music-MentalHealth\justgetstarted\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
   <si>
     <t>N/A</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Original Rating</t>
+  </si>
+  <si>
+    <t>Popularity</t>
+  </si>
+  <si>
+    <t>Pop Lower Range</t>
+  </si>
+  <si>
+    <t>Pop Upper Range</t>
   </si>
 </sst>
 </file>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,12 +535,12 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -556,8 +565,11 @@
       <c r="X2" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -615,8 +627,17 @@
       <c r="Z3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -627,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -674,8 +695,17 @@
       <c r="Z4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>51</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -733,8 +763,17 @@
       <c r="Z5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC5">
+        <v>52</v>
+      </c>
+      <c r="AD5">
+        <v>74</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -756,8 +795,17 @@
       <c r="Z6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>75</v>
+      </c>
+      <c r="AD6">
+        <v>100</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -768,7 +816,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X7">
         <v>131</v>
@@ -780,7 +828,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -791,10 +839,10 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -805,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X9" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
changed the cat for sunny
</commit_message>
<xml_diff>
--- a/Legend-for-Categorical-Variables.xlsx
+++ b/Legend-for-Categorical-Variables.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>N/A</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Pop Upper Range</t>
+  </si>
+  <si>
+    <t>Low-Health</t>
+  </si>
+  <si>
+    <t>Medium-Health</t>
+  </si>
+  <si>
+    <t>High-Health</t>
   </si>
 </sst>
 </file>
@@ -523,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -716,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -784,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="X6">
         <v>111</v>
@@ -816,7 +825,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="X7">
         <v>131</v>
@@ -839,7 +848,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -853,7 +862,7 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="X9" t="s">
         <v>38</v>

</xml_diff>